<commit_message>
[sourcestudy][doc][plans] add new plan
</commit_message>
<xml_diff>
--- a/doc/plans/tomcatplan.xlsx
+++ b/doc/plans/tomcatplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="7965"/>
+    <workbookView windowWidth="19095" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20">
   <si>
     <t>编号</t>
   </si>
@@ -46,12 +46,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t>《</t>
     </r>
     <r>
@@ -101,12 +95,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t>《</t>
     </r>
     <r>
@@ -137,6 +125,19 @@
       <t xml:space="preserve"> chapter7 Logger</t>
     </r>
   </si>
+  <si>
+    <t>1day</t>
+  </si>
+  <si>
+    <t>1.上一个计划未完成，延后到下一个
+时间点</t>
+  </si>
+  <si>
+    <t>《how tomcatw works》chapter8 loaders</t>
+  </si>
+  <si>
+    <t>《how tomcatw works》chapter9 manager</t>
+  </si>
 </sst>
 </file>
 
@@ -144,11 +145,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +166,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -173,9 +181,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
     <font>
@@ -200,22 +208,105 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,22 +322,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -261,93 +337,24 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -365,43 +372,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -413,13 +486,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,121 +546,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -575,25 +582,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -609,39 +607,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -663,6 +628,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -671,6 +654,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -679,10 +686,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -691,172 +698,175 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1201,13 +1211,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="1" width="5.875" customWidth="1"/>
     <col min="2" max="2" width="47.125" customWidth="1"/>
@@ -1219,51 +1229,51 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:9">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" ht="40" customHeight="1" spans="1:9">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="6">
         <v>42479</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="6">
         <v>42479</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="8" t="s">
@@ -1272,30 +1282,79 @@
       <c r="H2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="1" ht="40" customHeight="1" spans="1:9">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="6">
         <v>42480</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="6">
         <v>42480</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="11"/>
+      <c r="F3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" s="2" customFormat="1" ht="40" customHeight="1" spans="1:9">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="6">
+        <v>42486</v>
+      </c>
+      <c r="D4" s="6">
+        <v>42486</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" s="2" customFormat="1" ht="40" customHeight="1" spans="1:9">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="6">
+        <v>42487</v>
+      </c>
+      <c r="D5" s="6">
+        <v>42487</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[sourcestudt] add session manager
</commit_message>
<xml_diff>
--- a/doc/plans/tomcatplan.xlsx
+++ b/doc/plans/tomcatplan.xlsx
@@ -7,7 +7,7 @@
     <workbookView windowWidth="19095" windowHeight="7965"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="How tomcat to work" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37">
+  <si>
+    <t>how tomcat to work</t>
+  </si>
   <si>
     <t>编号</t>
   </si>
@@ -146,6 +149,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>《</t>
     </r>
     <r>
@@ -177,7 +186,24 @@
     </r>
   </si>
   <si>
-    <r>
+    <t>1.demo输出
+2.文档输出</t>
+  </si>
+  <si>
+    <t>10d</t>
+  </si>
+  <si>
+    <t>1.上一个计划未完成，延续到下一个任务点
+2.没有挤时间完成</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>《</t>
     </r>
     <r>
@@ -207,6 +233,13 @@
       </rPr>
       <t>chapter9 session manager</t>
     </r>
+  </si>
+  <si>
+    <t>1.demo输出
+2、文档输出</t>
+  </si>
+  <si>
+    <t>13d</t>
   </si>
   <si>
     <r>
@@ -634,10 +667,10 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -654,9 +687,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -687,15 +765,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -732,29 +826,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -838,7 +909,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -853,6 +924,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFD7E3BC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -877,30 +978,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1038,12 +1115,42 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF9BBB59"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF9BBB59"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9BBB59"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF9BBB59"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF9BBB59"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9BBB59"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1167,10 +1274,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1179,137 +1286,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1319,49 +1426,127 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1707,10 +1892,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1724,367 +1909,401 @@
     <col min="9" max="9" width="26.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:9">
-      <c r="A1" s="3" t="s">
+    <row r="1" ht="49" customHeight="1" spans="3:9">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="21" customHeight="1" spans="1:9">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="H2" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="I2" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" ht="40" customHeight="1" spans="1:9">
-      <c r="A2" s="4">
+    <row r="3" ht="40" customHeight="1" spans="1:9">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="6">
+      <c r="B3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8">
         <v>42479</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D3" s="8">
         <v>42479</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="F3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="G3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="H3" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" customFormat="1" ht="40" customHeight="1" spans="1:9">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="10" t="s">
+      <c r="I3" s="37" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" s="6">
-        <v>42480</v>
-      </c>
-      <c r="D3" s="6">
-        <v>42480</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="1" ht="40" customHeight="1" spans="1:9">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="12">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="14">
+        <v>42480</v>
+      </c>
+      <c r="D4" s="14">
+        <v>42480</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="6">
-        <v>42493</v>
-      </c>
-      <c r="D4" s="6">
-        <v>42493</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="16"/>
     </row>
     <row r="5" customFormat="1" ht="40" customHeight="1" spans="1:9">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="17">
+        <v>3</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="19">
         <v>42493</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="19">
         <v>42493</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="16"/>
+      <c r="E5" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="39" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" customFormat="1" ht="40" customHeight="1" spans="1:9">
-      <c r="A6" s="4">
+      <c r="A6" s="12">
+        <v>4</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="14">
+        <v>42493</v>
+      </c>
+      <c r="D6" s="14">
+        <v>42493</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customFormat="1" ht="40" customHeight="1" spans="1:9">
+      <c r="A7" s="17">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="6">
+      <c r="B7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="19">
         <v>42493</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D7" s="19">
         <v>42493</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="16"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="41"/>
     </row>
-    <row r="7" s="2" customFormat="1" ht="40" customHeight="1" spans="1:9">
-      <c r="A7" s="12">
+    <row r="8" s="2" customFormat="1" ht="40" customHeight="1" spans="1:9">
+      <c r="A8" s="27">
         <v>6</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="13">
+      <c r="B8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="28">
         <v>42494</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D8" s="28">
         <v>42494</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="17"/>
-    </row>
-    <row r="8" customFormat="1" ht="40" customHeight="1" spans="1:9">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="6">
-        <v>42494</v>
-      </c>
-      <c r="D8" s="6">
-        <v>42494</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="16"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="42"/>
     </row>
     <row r="9" customFormat="1" ht="40" customHeight="1" spans="1:9">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="6">
-        <v>42495</v>
-      </c>
-      <c r="D9" s="6">
-        <v>42495</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="16"/>
+      <c r="A9" s="17">
+        <v>7</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="19">
+        <v>42494</v>
+      </c>
+      <c r="D9" s="19">
+        <v>42494</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="41"/>
     </row>
     <row r="10" customFormat="1" ht="40" customHeight="1" spans="1:9">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="6">
+      <c r="A10" s="12">
+        <v>8</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="14">
         <v>42495</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="14">
         <v>42495</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="16"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="38"/>
     </row>
     <row r="11" customFormat="1" ht="40" customHeight="1" spans="1:9">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="6">
-        <v>42496</v>
-      </c>
-      <c r="D11" s="6">
-        <v>42496</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="16"/>
+      <c r="A11" s="17">
+        <v>9</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="19">
+        <v>42495</v>
+      </c>
+      <c r="D11" s="19">
+        <v>42495</v>
+      </c>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="41"/>
     </row>
     <row r="12" customFormat="1" ht="40" customHeight="1" spans="1:9">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="6">
+      <c r="A12" s="12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="14">
         <v>42496</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="14">
         <v>42496</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="16"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="38"/>
     </row>
     <row r="13" customFormat="1" ht="40" customHeight="1" spans="1:9">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="6">
+      <c r="A13" s="17">
+        <v>11</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="19">
         <v>42496</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="19">
         <v>42496</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="16"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="41"/>
     </row>
     <row r="14" customFormat="1" ht="40" customHeight="1" spans="1:9">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="6">
-        <v>42497</v>
-      </c>
-      <c r="D14" s="6">
-        <v>42497</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="16"/>
+      <c r="A14" s="12">
+        <v>12</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="14">
+        <v>42496</v>
+      </c>
+      <c r="D14" s="14">
+        <v>42496</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="38"/>
     </row>
     <row r="15" customFormat="1" ht="40" customHeight="1" spans="1:9">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="6">
+      <c r="A15" s="17">
+        <v>13</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="19">
         <v>42497</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="19">
         <v>42497</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="16"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="41"/>
     </row>
     <row r="16" customFormat="1" ht="40" customHeight="1" spans="1:9">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="6">
+      <c r="A16" s="12">
+        <v>14</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="14">
         <v>42497</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="14">
         <v>42497</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="16"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="38"/>
     </row>
     <row r="17" customFormat="1" ht="40" customHeight="1" spans="1:9">
-      <c r="A17" s="4">
-        <v>16</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="16"/>
+      <c r="A17" s="17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="19">
+        <v>42497</v>
+      </c>
+      <c r="D17" s="19">
+        <v>42497</v>
+      </c>
+      <c r="E17" s="25"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="41"/>
     </row>
     <row r="18" customFormat="1" ht="40" customHeight="1" spans="1:9">
-      <c r="A18" s="4">
+      <c r="A18" s="32">
+        <v>16</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="43"/>
+    </row>
+    <row r="19" customFormat="1" ht="40" customHeight="1" spans="1:9">
+      <c r="A19" s="32">
         <v>17</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="16"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="43"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:I1"/>
+  </mergeCells>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>